<commit_message>
BA Eval Prakualifikasi udah bisa download brur
</commit_message>
<xml_diff>
--- a/templates/BA Evaluasi Prakualifikasi.xlsx
+++ b/templates/BA Evaluasi Prakualifikasi.xlsx
@@ -57,6 +57,123 @@
       </rPr>
       <t>#namapengadaan#</t>
     </r>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Pemasukan Dokumen Prakualifikasi</t>
+  </si>
+  <si>
+    <t>a.</t>
+  </si>
+  <si>
+    <t>Yang mengambil Dokumen Prakualifikasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Penyedia Barang/Jasa</t>
+  </si>
+  <si>
+    <t>b.</t>
+  </si>
+  <si>
+    <t>Yang memasukan dokumen prakualifikasi</t>
+  </si>
+  <si>
+    <t>c.</t>
+  </si>
+  <si>
+    <t>Yang tidak memasukan dokumen prakualifikasi</t>
+  </si>
+  <si>
+    <t>Hasil Kualifikasi</t>
+  </si>
+  <si>
+    <t>Berdasarkan penilaian prakualifikasi yang diterima, maka calon penyedia barang/jasa  dibawah ini dinyatakan memenuhi persyaratan sesuai dengan Dokumen Prakualifikasi No.002/WEB/PPBJ-P.B/2012 sebagai berikut :</t>
+  </si>
+  <si>
+    <t>Yang memenuhi dokumen prakualifikasi</t>
+  </si>
+  <si>
+    <t>Yang tidak memenuhi dokumen prakualifikasi</t>
+  </si>
+  <si>
+    <t>Hasil prakualifikasi perusahaan sebagai berikut :</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Penyedia Jasa Konsultan</t>
+  </si>
+  <si>
+    <t>Administrasi</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Penilaian rinci kualifikasi terlampir</t>
+  </si>
+  <si>
+    <t>Demikian Berita Acara ini dibuat yang ditandantangani oleh seluruh anggota panitia pengadaan barang/jasa.</t>
+  </si>
+  <si>
+    <t>Disahkan oleh :</t>
+  </si>
+  <si>
+    <t>.................. /</t>
+  </si>
+  <si>
+    <t>Ketua merangkap Anggota</t>
+  </si>
+  <si>
+    <t>…………………………</t>
+  </si>
+  <si>
+    <t>............/</t>
+  </si>
+  <si>
+    <t>Sekretaris merangkap Anggota</t>
+  </si>
+  <si>
+    <t>..............</t>
+  </si>
+  <si>
+    <t>............</t>
+  </si>
+  <si>
+    <t>Anggota</t>
+  </si>
+  <si>
+    <t>#mengambil#</t>
+  </si>
+  <si>
+    <t>#memasukkan#</t>
+  </si>
+  <si>
+    <t>#tidakmemasukkan#</t>
+  </si>
+  <si>
+    <t>#memenuhi#</t>
+  </si>
+  <si>
+    <t>#tidakmemenuhi#</t>
+  </si>
+  <si>
+    <t>#KDIVMUM/MSDAF#</t>
   </si>
   <si>
     <r>
@@ -137,7 +254,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>#panitia#</t>
+      <t>#namapanitia#</t>
     </r>
     <r>
       <rPr>
@@ -154,7 +271,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>...........</t>
+      <t>#metodepengadaan#</t>
     </r>
     <r>
       <rPr>
@@ -162,41 +279,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">(metode) sesuai Surat Tugas Kepala Divisi Umum dan Manajemen Kantor Pusat No. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#nosk#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tanggal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#tglsk#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> telah melakukan kualifikasi terhadap dokumen prakualikasi yang disampaikan Penyedia Barang/Jasa sesuai Dokumen Prakualifikasi No </t>
+      <t xml:space="preserve">(metode) #kalimatpanitia# telah melakukan kualifikasi terhadap dokumen prakualikasi yang disampaikan Penyedia Barang/Jasa sesuai Dokumen Prakualifikasi No </t>
     </r>
     <r>
       <rPr>
@@ -234,105 +317,6 @@
     </r>
   </si>
   <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>Pemasukan Dokumen Prakualifikasi</t>
-  </si>
-  <si>
-    <t>a.</t>
-  </si>
-  <si>
-    <t>Yang mengambil Dokumen Prakualifikasi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Penyedia Barang/Jasa</t>
-  </si>
-  <si>
-    <t>b.</t>
-  </si>
-  <si>
-    <t>Yang memasukan dokumen prakualifikasi</t>
-  </si>
-  <si>
-    <t>c.</t>
-  </si>
-  <si>
-    <t>Yang tidak memasukan dokumen prakualifikasi</t>
-  </si>
-  <si>
-    <t>Hasil Kualifikasi</t>
-  </si>
-  <si>
-    <t>Berdasarkan penilaian prakualifikasi yang diterima, maka calon penyedia barang/jasa  dibawah ini dinyatakan memenuhi persyaratan sesuai dengan Dokumen Prakualifikasi No.002/WEB/PPBJ-P.B/2012 sebagai berikut :</t>
-  </si>
-  <si>
-    <t>Yang memenuhi dokumen prakualifikasi</t>
-  </si>
-  <si>
-    <t>Yang tidak memenuhi dokumen prakualifikasi</t>
-  </si>
-  <si>
-    <t>Hasil prakualifikasi perusahaan sebagai berikut :</t>
-  </si>
-  <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Penyedia Jasa Konsultan</t>
-  </si>
-  <si>
-    <t>Administrasi</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Penilaian rinci kualifikasi terlampir</t>
-  </si>
-  <si>
-    <t>Demikian Berita Acara ini dibuat yang ditandantangani oleh seluruh anggota panitia pengadaan barang/jasa.</t>
-  </si>
-  <si>
-    <t>Disahkan oleh :</t>
-  </si>
-  <si>
-    <t>.................. /</t>
-  </si>
-  <si>
-    <t>Ketua merangkap Anggota</t>
-  </si>
-  <si>
-    <t>…………………………</t>
-  </si>
-  <si>
-    <t>............/</t>
-  </si>
-  <si>
-    <t>Sekretaris merangkap Anggota</t>
-  </si>
-  <si>
-    <t>..............</t>
-  </si>
-  <si>
-    <t>............</t>
-  </si>
-  <si>
-    <t>Anggota</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -357,26 +341,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>#namapengadaan#</t>
+      <t>#namapengadaan2#</t>
     </r>
-  </si>
-  <si>
-    <t>#mengambil#</t>
-  </si>
-  <si>
-    <t>#memasukkan#</t>
-  </si>
-  <si>
-    <t>#tidakmemasukkan#</t>
-  </si>
-  <si>
-    <t>#memenuhi#</t>
-  </si>
-  <si>
-    <t>#tidakmemenuhi#</t>
-  </si>
-  <si>
-    <t>#KDIVMUM/MSDAF#</t>
   </si>
 </sst>
 </file>
@@ -682,74 +648,74 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1211,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28:K28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1235,41 +1201,41 @@
     </row>
     <row r="7" spans="1:15" ht="18">
       <c r="A7" s="4"/>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="4"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="4"/>
@@ -1290,104 +1256,104 @@
     </row>
     <row r="10" spans="1:15" ht="17">
       <c r="A10" s="4"/>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
     </row>
     <row r="11" spans="1:15" ht="15">
       <c r="A11" s="4"/>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="4"/>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+    </row>
+    <row r="15" spans="1:15" ht="57" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
+      <c r="B15" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
     </row>
     <row r="16" spans="1:15" ht="15">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1406,24 +1372,24 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="63" t="s">
-        <v>40</v>
+      <c r="K17" s="42" t="s">
+        <v>38</v>
       </c>
       <c r="L17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
@@ -1433,24 +1399,24 @@
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="63" t="s">
-        <v>41</v>
+      <c r="K18" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="L18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -1460,22 +1426,22 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="63" t="s">
-        <v>42</v>
+      <c r="K19" s="42" t="s">
+        <v>40</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -1504,7 +1470,7 @@
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1522,42 +1488,42 @@
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
+      <c r="D22" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
     </row>
     <row r="23" spans="1:15" ht="15">
       <c r="A23" s="4"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="63" t="s">
-        <v>43</v>
+      <c r="K23" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="L23" s="14"/>
       <c r="M23" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
@@ -1567,22 +1533,22 @@
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="63" t="s">
-        <v>44</v>
+      <c r="K24" s="42" t="s">
+        <v>42</v>
       </c>
       <c r="L24" s="14"/>
       <c r="M24" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
@@ -1592,7 +1558,7 @@
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="9"/>
@@ -1628,17 +1594,17 @@
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="54"/>
       <c r="F27" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="56"/>
       <c r="H27" s="56"/>
       <c r="I27" s="57"/>
       <c r="J27" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K27" s="57"/>
       <c r="L27" s="17"/>
@@ -1651,14 +1617,14 @@
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="20"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
       <c r="I28" s="44"/>
-      <c r="J28" s="42"/>
+      <c r="J28" s="43"/>
       <c r="K28" s="44"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
@@ -1670,14 +1636,14 @@
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" s="22"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
       <c r="I29" s="44"/>
-      <c r="J29" s="42"/>
+      <c r="J29" s="43"/>
       <c r="K29" s="44"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
@@ -1689,14 +1655,14 @@
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="22"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
       <c r="I30" s="44"/>
-      <c r="J30" s="42"/>
+      <c r="J30" s="43"/>
       <c r="K30" s="44"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -1708,14 +1674,14 @@
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" s="22"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
       <c r="I31" s="44"/>
-      <c r="J31" s="42"/>
+      <c r="J31" s="43"/>
       <c r="K31" s="44"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -1727,14 +1693,14 @@
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="22"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
       <c r="I32" s="44"/>
-      <c r="J32" s="42"/>
+      <c r="J32" s="43"/>
       <c r="K32" s="44"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -1763,7 +1729,7 @@
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
       <c r="D34" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
@@ -1824,11 +1790,11 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="52" t="s">
+      <c r="M37" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="N37" s="52"/>
-      <c r="O37" s="52"/>
+      <c r="N37" s="64"/>
+      <c r="O37" s="64"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="4"/>
@@ -1842,13 +1808,13 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="45" t="str">
+      <c r="L38" s="63" t="str">
         <f>B8</f>
         <v>No. #nobapq#</v>
       </c>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="63"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="4"/>
@@ -1886,22 +1852,22 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="4"/>
-      <c r="B41" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="47"/>
+      <c r="B41" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="52"/>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="4"/>
@@ -1926,16 +1892,16 @@
       <c r="E43" s="32"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
-      <c r="H43" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
+      <c r="H43" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="4"/>
@@ -1945,30 +1911,30 @@
       <c r="E44" s="32"/>
       <c r="F44" s="32"/>
       <c r="G44" s="32"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="48"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="9"/>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="34" t="s">
         <v>30</v>
-      </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I45" s="34" t="s">
-        <v>31</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="35"/>
@@ -1987,13 +1953,13 @@
       <c r="G46" s="35"/>
       <c r="H46" s="35"/>
       <c r="I46" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="35"/>
       <c r="M46" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N46" s="35"/>
       <c r="O46" s="35"/>
@@ -2041,10 +2007,10 @@
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
       <c r="H49" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I49" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J49" s="37"/>
       <c r="K49" s="37"/>
@@ -2063,27 +2029,27 @@
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J50" s="37"/>
       <c r="K50" s="37"/>
       <c r="L50" s="37"/>
       <c r="M50" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N50" s="37"/>
       <c r="O50" s="37"/>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="37"/>
-      <c r="B51" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
+      <c r="B51" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
       <c r="H51" s="37"/>
       <c r="I51" s="37"/>
       <c r="J51" s="37"/>
@@ -2095,14 +2061,14 @@
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="37"/>
-      <c r="B52" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
+      <c r="B52" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
       <c r="H52" s="37"/>
       <c r="I52" s="37"/>
       <c r="J52" s="37"/>
@@ -2121,10 +2087,10 @@
       <c r="F53" s="37"/>
       <c r="G53" s="37"/>
       <c r="H53" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I53" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J53" s="37"/>
       <c r="K53" s="37"/>
@@ -2143,13 +2109,13 @@
       <c r="G54" s="37"/>
       <c r="H54" s="37"/>
       <c r="I54" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J54" s="37"/>
       <c r="K54" s="37"/>
       <c r="L54" s="37"/>
       <c r="M54" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N54" s="37"/>
       <c r="O54" s="37"/>
@@ -2428,6 +2394,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="H43:O44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="F29:I29"/>
@@ -2442,19 +2421,6 @@
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="H43:O44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="M37:O37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>